<commit_message>
Gestion de eventos SNTP Cambios: -Gestion de eventos SNTP -Inclusion en la pagin ade Info sobre la hora actual y los eventos de sincronizacion
</commit_message>
<xml_diff>
--- a/Configuraciones/Navidad/Secuenciador.xlsx
+++ b/Configuraciones/Navidad/Secuenciador.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\arduino\desarrollos\Sketchs\Actuador\data\Navidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\arduino\desarrollos\Sketchs\Actuador\Actuador\Configuraciones\Navidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C8F8F7-23B4-44E5-9D3B-8DBC13D1E191}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B43B6A3-B32D-4DA7-9CDA-297AEA7B7C74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="3855" xr2:uid="{E272C0E1-DFCC-4036-ADAB-96F87FDBC628}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E272C0E1-DFCC-4036-ADAB-96F87FDBC628}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5727D02F-810E-4AAF-AB01-9DED2FEDECD7}">
   <dimension ref="A1:AB42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -666,7 +666,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -720,7 +720,7 @@
         <v>0</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3">
         <v>1</v>
@@ -755,7 +755,7 @@
         <v>4</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -809,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4">
         <v>1</v>
@@ -844,7 +844,7 @@
         <v>8</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -933,7 +933,7 @@
         <v>16</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1022,7 +1022,7 @@
         <v>32</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1111,7 +1111,7 @@
         <v>64</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1200,7 +1200,7 @@
         <v>128</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1289,7 +1289,7 @@
         <v>256</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1378,7 +1378,7 @@
         <v>512</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1467,7 +1467,7 @@
         <v>1024</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1556,7 +1556,7 @@
         <v>2048</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1631,7 +1631,7 @@
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E14">
         <f>+SUMPRODUCT($D$2:$D$13,E2:E13)</f>
-        <v>4095</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <f t="shared" ref="F14:N14" si="3">+SUMPRODUCT($D$2:$D$13,F2:F13)</f>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="W14">
         <f t="shared" ref="W14" si="11">+SUMPRODUCT($D$2:$D$13,W2:W13)</f>
-        <v>4088</v>
+        <v>4095</v>
       </c>
       <c r="X14">
         <f t="shared" ref="X14" si="12">+SUMPRODUCT($D$2:$D$13,X2:X13)</f>

</xml_diff>